<commit_message>
Disability Labour Force Participation widget.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
+++ b/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -320,10 +320,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -333,7 +333,7 @@
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -350,7 +350,6 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -367,51 +366,49 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="F3" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="n">
         <v>2013</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
@@ -419,123 +416,119 @@
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6"/>
       <c r="C5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="n">
+        <v>3323</v>
+      </c>
       <c r="F5" s="10" t="n">
-        <v>3323</v>
+        <v>3170</v>
       </c>
       <c r="G5" s="10" t="n">
-        <v>3170</v>
+        <v>2209</v>
       </c>
       <c r="H5" s="10" t="n">
-        <v>2209</v>
+        <v>928</v>
       </c>
       <c r="I5" s="10" t="n">
-        <v>928</v>
+        <v>1030</v>
       </c>
       <c r="J5" s="10" t="n">
-        <v>1030</v>
+        <v>197</v>
       </c>
       <c r="K5" s="10" t="n">
-        <v>197</v>
+        <v>261</v>
       </c>
       <c r="L5" s="10" t="n">
-        <v>261</v>
+        <v>149</v>
       </c>
       <c r="M5" s="10" t="n">
-        <v>149</v>
-      </c>
-      <c r="N5" s="10" t="n">
         <v>11266</v>
       </c>
-      <c r="O5" s="3"/>
+      <c r="N5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="6"/>
       <c r="C6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="n">
+        <v>282</v>
+      </c>
       <c r="F6" s="10" t="n">
-        <v>282</v>
+        <v>165</v>
       </c>
       <c r="G6" s="10" t="n">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="H6" s="10" t="n">
-        <v>121</v>
+        <v>28</v>
       </c>
       <c r="I6" s="10" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J6" s="10" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="K6" s="10" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="L6" s="10" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="M6" s="10" t="n">
-        <v>37</v>
-      </c>
-      <c r="N6" s="10" t="n">
         <v>710</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="N6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="n">
+        <v>204</v>
+      </c>
       <c r="F7" s="10" t="n">
-        <v>204</v>
+        <v>392</v>
       </c>
       <c r="G7" s="10" t="n">
-        <v>392</v>
+        <v>206</v>
       </c>
       <c r="H7" s="10" t="n">
-        <v>206</v>
+        <v>9</v>
       </c>
       <c r="I7" s="10" t="n">
+        <v>60</v>
+      </c>
+      <c r="J7" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="J7" s="10" t="n">
-        <v>60</v>
-      </c>
       <c r="K7" s="10" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="L7" s="10" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="M7" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="N7" s="10" t="n">
         <v>902</v>
       </c>
-      <c r="O7" s="3"/>
+      <c r="N7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="3"/>
       <c r="C8" s="8"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -543,17 +536,16 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="B9" s="11"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
@@ -561,121 +553,117 @@
       <c r="J9" s="10"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
+      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="6"/>
       <c r="C10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10" t="n">
+        <v>1576</v>
+      </c>
       <c r="F10" s="10" t="n">
-        <v>1576</v>
+        <v>808</v>
       </c>
       <c r="G10" s="10" t="n">
-        <v>808</v>
+        <v>685</v>
       </c>
       <c r="H10" s="10" t="n">
-        <v>685</v>
+        <v>663</v>
       </c>
       <c r="I10" s="10" t="n">
-        <v>663</v>
+        <v>698</v>
       </c>
       <c r="J10" s="10" t="n">
-        <v>698</v>
+        <v>27</v>
       </c>
       <c r="K10" s="10" t="n">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="L10" s="10" t="n">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="M10" s="10" t="n">
-        <v>58</v>
-      </c>
-      <c r="N10" s="10" t="n">
         <v>4606</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="N10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="6"/>
       <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="n">
+        <v>1483</v>
+      </c>
       <c r="F11" s="10" t="n">
-        <v>1483</v>
+        <v>657</v>
       </c>
       <c r="G11" s="10" t="n">
-        <v>657</v>
+        <v>582</v>
       </c>
       <c r="H11" s="10" t="n">
-        <v>582</v>
+        <v>183</v>
       </c>
       <c r="I11" s="10" t="n">
-        <v>183</v>
+        <v>142</v>
       </c>
       <c r="J11" s="10" t="n">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="K11" s="10" t="n">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="L11" s="10" t="n">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="M11" s="10" t="n">
-        <v>132</v>
-      </c>
-      <c r="N11" s="10" t="n">
         <v>3385</v>
       </c>
-      <c r="O11" s="3"/>
+      <c r="N11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3"/>
       <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="n">
+        <v>2096</v>
+      </c>
       <c r="F12" s="10" t="n">
-        <v>2096</v>
+        <v>2533</v>
       </c>
       <c r="G12" s="10" t="n">
-        <v>2533</v>
+        <v>1535</v>
       </c>
       <c r="H12" s="10" t="n">
-        <v>1535</v>
+        <v>265</v>
       </c>
       <c r="I12" s="10" t="n">
-        <v>265</v>
+        <v>312</v>
       </c>
       <c r="J12" s="10" t="n">
-        <v>312</v>
+        <v>119</v>
       </c>
       <c r="K12" s="10" t="n">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="L12" s="10" t="n">
-        <v>128</v>
+        <v>34</v>
       </c>
       <c r="M12" s="10" t="n">
-        <v>34</v>
-      </c>
-      <c r="N12" s="10" t="n">
         <v>7022</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="N12" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A1:N1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -694,7 +682,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Misc last minute typo corrections.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
+++ b/dashboard_loader/education_ecenqs_uploader/education_ecenqs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
-    <t xml:space="preserve">The proportion of early childhood education and care services in Australia with a quality rating, by quality rating level and jurisdiction, March 2013 and September 2015</t>
+    <t xml:space="preserve">The proportion of early childhood education and care services in Australia with a quality rating, by quality rating level and jurisdiction, March 2013 and September 2016</t>
   </si>
   <si>
     <t xml:space="preserve">NSW</t>
@@ -119,7 +119,7 @@
     <numFmt numFmtId="165" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -269,13 +269,6 @@
       <color rgb="FF00000A"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF00000A"/>
-      <name val=""/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -426,7 +419,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -484,10 +477,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -594,14 +583,14 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -811,9 +800,9 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="n">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B9" s="11"/>
       <c r="D9" s="12"/>
@@ -954,7 +943,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -977,7 +966,7 @@
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>16</v>
       </c>
     </row>
@@ -985,7 +974,7 @@
       <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -993,7 +982,7 @@
       <c r="A4" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="16" t="n">
+      <c r="B4" s="15" t="n">
         <v>2015</v>
       </c>
     </row>
@@ -1001,18 +990,18 @@
       <c r="A5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="52.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13"/>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="26.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1020,13 +1009,13 @@
       <c r="A8" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="39.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1034,7 +1023,7 @@
       <c r="A10" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>